<commit_message>
Added excel files to Project Team 6 GitHub
</commit_message>
<xml_diff>
--- a/Covid vs Population.xlsx
+++ b/Covid vs Population.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rober\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rober\Desktop\ClassHomework\Project-One-Team6\Team6_Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07CDE4F5-78F6-4EF7-9825-ACD16C32BC6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7366750-4DA5-45A8-BCF3-A844D4663584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29985" yWindow="105" windowWidth="22620" windowHeight="15225" xr2:uid="{F9319FF3-4BE5-4CF7-9F4A-32D15067C69B}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -388,18 +388,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -410,12 +410,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,6 +425,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -742,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D88864-7A2F-468C-B379-1D5AF09F0955}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -886,14 +887,14 @@
         <v>0.40511035915559268</v>
       </c>
       <c r="F9" s="6">
-        <f>B9/J9</f>
+        <f t="shared" ref="F9:F40" si="1">B9/J9</f>
         <v>1.0401395151526436E-2</v>
       </c>
       <c r="G9" s="2">
         <v>499143</v>
       </c>
       <c r="H9" s="6">
-        <f>G9/J9</f>
+        <f t="shared" ref="H9:H40" si="2">G9/J9</f>
         <v>2.567546081321392E-2</v>
       </c>
       <c r="I9" s="1">
@@ -916,18 +917,18 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="22">
-        <f t="shared" ref="E10:E60" si="1">B10/G10</f>
+        <f t="shared" ref="E10:E60" si="3">B10/G10</f>
         <v>0.10516290973521016</v>
       </c>
       <c r="F10" s="6">
-        <f>B10/J10</f>
+        <f t="shared" si="1"/>
         <v>9.715370605672672E-4</v>
       </c>
       <c r="G10" s="2">
         <v>203180</v>
       </c>
       <c r="H10" s="6">
-        <f>G10/J10</f>
+        <f t="shared" si="2"/>
         <v>9.2384003353796675E-3</v>
       </c>
       <c r="I10" s="1">
@@ -950,18 +951,18 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="22">
+        <f t="shared" si="3"/>
+        <v>0.11541580946352271</v>
+      </c>
+      <c r="F11" s="6">
         <f t="shared" si="1"/>
-        <v>0.11541580946352271</v>
-      </c>
-      <c r="F11" s="6">
-        <f>B11/J11</f>
         <v>5.8436322824401902E-4</v>
       </c>
       <c r="G11" s="2">
         <v>202208</v>
       </c>
       <c r="H11" s="6">
-        <f>G11/J11</f>
+        <f t="shared" si="2"/>
         <v>5.063112505646011E-3</v>
       </c>
       <c r="I11" s="1">
@@ -984,18 +985,18 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="22">
+        <f t="shared" si="3"/>
+        <v>9.9845016283531443E-2</v>
+      </c>
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
-        <v>9.9845016283531443E-2</v>
-      </c>
-      <c r="F12" s="6">
-        <f>B12/J12</f>
         <v>4.9619481618245207E-4</v>
       </c>
       <c r="G12" s="2">
         <v>146467</v>
       </c>
       <c r="H12" s="6">
-        <f>G12/J12</f>
+        <f t="shared" si="2"/>
         <v>4.9696503105713351E-3</v>
       </c>
       <c r="I12" s="1">
@@ -1018,18 +1019,18 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="22">
+        <f t="shared" si="3"/>
+        <v>0.49239486599796817</v>
+      </c>
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
-        <v>0.49239486599796817</v>
-      </c>
-      <c r="F13" s="6">
-        <f>B13/J13</f>
         <v>7.7013853407357225E-3</v>
       </c>
       <c r="G13" s="2">
         <v>139774</v>
       </c>
       <c r="H13" s="6">
-        <f>G13/J13</f>
+        <f t="shared" si="2"/>
         <v>1.564066945565493E-2</v>
       </c>
       <c r="I13" s="1">
@@ -1052,18 +1053,18 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="22">
+        <f t="shared" si="3"/>
+        <v>0.18966407495266815</v>
+      </c>
+      <c r="F14" s="6">
         <f t="shared" si="1"/>
-        <v>0.18966407495266815</v>
-      </c>
-      <c r="F14" s="6">
-        <f>B14/J14</f>
         <v>1.9768536912994571E-3</v>
       </c>
       <c r="G14" s="2">
         <v>133631</v>
       </c>
       <c r="H14" s="6">
-        <f>G14/J14</f>
+        <f t="shared" si="2"/>
         <v>1.0422921113515003E-2</v>
       </c>
       <c r="I14" s="1">
@@ -1086,18 +1087,18 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="22">
+        <f t="shared" si="3"/>
+        <v>0.22254269029877283</v>
+      </c>
+      <c r="F15" s="6">
         <f t="shared" si="1"/>
-        <v>0.22254269029877283</v>
-      </c>
-      <c r="F15" s="6">
-        <f>B15/J15</f>
         <v>4.0367818293073256E-3</v>
       </c>
       <c r="G15" s="2">
         <v>126551</v>
       </c>
       <c r="H15" s="6">
-        <f>G15/J15</f>
+        <f t="shared" si="2"/>
         <v>1.8139359346684352E-2</v>
       </c>
       <c r="I15" s="1">
@@ -1120,18 +1121,18 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="22">
+        <f t="shared" si="3"/>
+        <v>0.1817061019067403</v>
+      </c>
+      <c r="F16" s="6">
         <f t="shared" si="1"/>
-        <v>0.1817061019067403</v>
-      </c>
-      <c r="F16" s="6">
-        <f>B16/J16</f>
         <v>4.6323245753020761E-3</v>
       </c>
       <c r="G16" s="2">
         <v>118422</v>
       </c>
       <c r="H16" s="6">
-        <f>G16/J16</f>
+        <f t="shared" si="2"/>
         <v>2.5493500365109327E-2</v>
       </c>
       <c r="I16" s="1">
@@ -1154,18 +1155,18 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="22">
+        <f t="shared" si="3"/>
+        <v>0.21015947060099804</v>
+      </c>
+      <c r="F17" s="6">
         <f t="shared" si="1"/>
-        <v>0.21015947060099804</v>
-      </c>
-      <c r="F17" s="6">
-        <f>B17/J17</f>
         <v>1.8363020492931812E-3</v>
       </c>
       <c r="G17" s="2">
         <v>110616</v>
       </c>
       <c r="H17" s="6">
-        <f>G17/J17</f>
+        <f t="shared" si="2"/>
         <v>8.7376602350675153E-3</v>
       </c>
       <c r="I17" s="1">
@@ -1188,18 +1189,18 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="22">
+        <f t="shared" si="3"/>
+        <v>0.11219112308232815</v>
+      </c>
+      <c r="F18" s="6">
         <f t="shared" si="1"/>
-        <v>0.11219112308232815</v>
-      </c>
-      <c r="F18" s="6">
-        <f>B18/J18</f>
         <v>1.3515289989412724E-3</v>
       </c>
       <c r="G18" s="2">
         <v>93929</v>
       </c>
       <c r="H18" s="6">
-        <f>G18/J18</f>
+        <f t="shared" si="2"/>
         <v>1.2046666098078836E-2</v>
       </c>
       <c r="I18" s="1">
@@ -1222,18 +1223,18 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="22">
+        <f t="shared" si="3"/>
+        <v>0.31314220768677659</v>
+      </c>
+      <c r="F19" s="6">
         <f t="shared" si="1"/>
-        <v>0.31314220768677659</v>
-      </c>
-      <c r="F19" s="6">
-        <f>B19/J19</f>
         <v>2.6879962218127993E-3</v>
       </c>
       <c r="G19" s="2">
         <v>86226</v>
       </c>
       <c r="H19" s="6">
-        <f>G19/J19</f>
+        <f t="shared" si="2"/>
         <v>8.5839473435069223E-3</v>
       </c>
       <c r="I19" s="1">
@@ -1256,18 +1257,18 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="22">
+        <f t="shared" si="3"/>
+        <v>7.3866879780796896E-2</v>
+      </c>
+      <c r="F20" s="6">
         <f t="shared" si="1"/>
-        <v>7.3866879780796896E-2</v>
-      </c>
-      <c r="F20" s="6">
-        <f>B20/J20</f>
         <v>8.4420961798753653E-4</v>
       </c>
       <c r="G20" s="2">
         <v>78831</v>
       </c>
       <c r="H20" s="6">
-        <f>G20/J20</f>
+        <f t="shared" si="2"/>
         <v>1.1428797594981194E-2</v>
       </c>
       <c r="I20" s="1">
@@ -1290,18 +1291,18 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="22">
+        <f t="shared" si="3"/>
+        <v>0.10538645136576598</v>
+      </c>
+      <c r="F21" s="6">
         <f t="shared" si="1"/>
-        <v>0.10538645136576598</v>
-      </c>
-      <c r="F21" s="6">
-        <f>B21/J21</f>
         <v>6.0888545445599788E-4</v>
       </c>
       <c r="G21" s="2">
         <v>67874</v>
       </c>
       <c r="H21" s="6">
-        <f>G21/J21</f>
+        <f t="shared" si="2"/>
         <v>5.7776445317693839E-3</v>
       </c>
       <c r="I21" s="1">
@@ -1324,18 +1325,18 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="22">
+        <f t="shared" si="3"/>
+        <v>7.7245960116237952E-2</v>
+      </c>
+      <c r="F22" s="6">
         <f t="shared" si="1"/>
-        <v>7.7245960116237952E-2</v>
-      </c>
-      <c r="F22" s="6">
-        <f>B22/J22</f>
         <v>4.73432466422952E-4</v>
       </c>
       <c r="G22" s="2">
         <v>65039</v>
       </c>
       <c r="H22" s="6">
-        <f>G22/J22</f>
+        <f t="shared" si="2"/>
         <v>6.1288961352870966E-3</v>
       </c>
       <c r="I22" s="1">
@@ -1358,18 +1359,18 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="22">
+        <f t="shared" si="3"/>
+        <v>0.23016425277125982</v>
+      </c>
+      <c r="F23" s="6">
         <f t="shared" si="1"/>
-        <v>0.23016425277125982</v>
-      </c>
-      <c r="F23" s="6">
-        <f>B23/J23</f>
         <v>1.3247878015573498E-3</v>
       </c>
       <c r="G23" s="2">
         <v>61795</v>
       </c>
       <c r="H23" s="6">
-        <f>G23/J23</f>
+        <f t="shared" si="2"/>
         <v>5.755836475935909E-3</v>
       </c>
       <c r="I23" s="1">
@@ -1392,18 +1393,18 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="22">
+        <f t="shared" si="3"/>
+        <v>0.17627900917499489</v>
+      </c>
+      <c r="F24" s="6">
         <f t="shared" si="1"/>
-        <v>0.17627900917499489</v>
-      </c>
-      <c r="F24" s="6">
-        <f>B24/J24</f>
         <v>1.5570967247706604E-3</v>
       </c>
       <c r="G24" s="2">
         <v>53733</v>
       </c>
       <c r="H24" s="6">
-        <f>G24/J24</f>
+        <f t="shared" si="2"/>
         <v>8.8331374907202158E-3</v>
       </c>
       <c r="I24" s="1">
@@ -1426,18 +1427,18 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="22">
+        <f t="shared" si="3"/>
+        <v>9.7669765309100001E-2</v>
+      </c>
+      <c r="F25" s="6">
         <f t="shared" si="1"/>
-        <v>9.7669765309100001E-2</v>
-      </c>
-      <c r="F25" s="6">
-        <f>B25/J25</f>
         <v>7.5957122965926275E-4</v>
       </c>
       <c r="G25" s="2">
         <v>47978</v>
       </c>
       <c r="H25" s="6">
-        <f>G25/J25</f>
+        <f t="shared" si="2"/>
         <v>7.7769330893282347E-3</v>
       </c>
       <c r="I25" s="1">
@@ -1460,18 +1461,18 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="22">
+        <f t="shared" si="3"/>
+        <v>5.1897753679318356E-2</v>
+      </c>
+      <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>5.1897753679318356E-2</v>
-      </c>
-      <c r="F26" s="6">
-        <f>B26/J26</f>
         <v>7.3489198276111597E-4</v>
       </c>
       <c r="G26" s="2">
         <v>46476</v>
       </c>
       <c r="H26" s="6">
-        <f>G26/J26</f>
+        <f t="shared" si="2"/>
         <v>1.4160381339471652E-2</v>
       </c>
       <c r="I26" s="1">
@@ -1494,18 +1495,18 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="22">
+        <f t="shared" si="3"/>
+        <v>0.18530108438185888</v>
+      </c>
+      <c r="F27" s="6">
         <f t="shared" si="1"/>
-        <v>0.18530108438185888</v>
-      </c>
-      <c r="F27" s="6">
-        <f>B27/J27</f>
         <v>1.264129354812216E-3</v>
       </c>
       <c r="G27" s="2">
         <v>46017</v>
       </c>
       <c r="H27" s="6">
-        <f>G27/J27</f>
+        <f t="shared" si="2"/>
         <v>6.8220289105657018E-3</v>
       </c>
       <c r="I27" s="1">
@@ -1528,18 +1529,18 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="22">
+        <f t="shared" si="3"/>
+        <v>0.30516349992364916</v>
+      </c>
+      <c r="F28" s="6">
         <f t="shared" si="1"/>
-        <v>0.30516349992364916</v>
-      </c>
-      <c r="F28" s="6">
-        <f>B28/J28</f>
         <v>3.926100951509047E-3</v>
       </c>
       <c r="G28" s="2">
         <v>45841</v>
       </c>
       <c r="H28" s="6">
-        <f>G28/J28</f>
+        <f t="shared" si="2"/>
         <v>1.2865565352643235E-2</v>
       </c>
       <c r="I28" s="1">
@@ -1562,18 +1563,18 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="22">
+        <f t="shared" si="3"/>
+        <v>8.6311683599419445E-2</v>
+      </c>
+      <c r="F29" s="6">
         <f t="shared" si="1"/>
-        <v>8.6311683599419445E-2</v>
-      </c>
-      <c r="F29" s="6">
-        <f>B29/J29</f>
         <v>5.1582341870847902E-4</v>
       </c>
       <c r="G29" s="2">
         <v>44096</v>
       </c>
       <c r="H29" s="6">
-        <f>G29/J29</f>
+        <f t="shared" si="2"/>
         <v>5.976287301988726E-3</v>
       </c>
       <c r="I29" s="1">
@@ -1596,18 +1597,18 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="22">
+        <f t="shared" si="3"/>
+        <v>0.14430699436428687</v>
+      </c>
+      <c r="F30" s="6">
         <f t="shared" si="1"/>
-        <v>0.14430699436428687</v>
-      </c>
-      <c r="F30" s="6">
-        <f>B30/J30</f>
         <v>7.1537814939984636E-4</v>
       </c>
       <c r="G30" s="2">
         <v>42763</v>
       </c>
       <c r="H30" s="6">
-        <f>G30/J30</f>
+        <f t="shared" si="2"/>
         <v>4.957335245954566E-3</v>
       </c>
       <c r="I30" s="1">
@@ -1630,18 +1631,18 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="22">
+        <f t="shared" si="3"/>
+        <v>8.5555448594532152E-2</v>
+      </c>
+      <c r="F31" s="6">
         <f t="shared" si="1"/>
-        <v>8.5555448594532152E-2</v>
-      </c>
-      <c r="F31" s="6">
-        <f>B31/J31</f>
         <v>6.0751015849265023E-4</v>
       </c>
       <c r="G31" s="2">
         <v>41552</v>
       </c>
       <c r="H31" s="6">
-        <f>G31/J31</f>
+        <f t="shared" si="2"/>
         <v>7.1007769636249234E-3</v>
       </c>
       <c r="I31" s="1">
@@ -1663,19 +1664,19 @@
       </c>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
-      <c r="E32" s="22">
+      <c r="E32" s="24">
+        <f t="shared" si="3"/>
+        <v>4.3194617874162226E-2</v>
+      </c>
+      <c r="F32" s="17">
         <f t="shared" si="1"/>
-        <v>4.3194617874162226E-2</v>
-      </c>
-      <c r="F32" s="17">
-        <f>B32/J32</f>
         <v>2.9733341917118175E-4</v>
       </c>
       <c r="G32" s="16">
         <v>39241</v>
       </c>
       <c r="H32" s="17">
-        <f>G32/J32</f>
+        <f t="shared" si="2"/>
         <v>6.8835756352190825E-3</v>
       </c>
       <c r="I32" s="15">
@@ -1698,18 +1699,18 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="22">
+        <f t="shared" si="3"/>
+        <v>0.19851840379949409</v>
+      </c>
+      <c r="F33" s="6">
         <f t="shared" si="1"/>
-        <v>0.19851840379949409</v>
-      </c>
-      <c r="F33" s="6">
-        <f>B33/J33</f>
         <v>1.3157070894903213E-3</v>
       </c>
       <c r="G33" s="2">
         <v>38742</v>
       </c>
       <c r="H33" s="6">
-        <f>G33/J33</f>
+        <f t="shared" si="2"/>
         <v>6.6276328255147612E-3</v>
       </c>
       <c r="I33" s="1">
@@ -1732,18 +1733,18 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="22">
+        <f t="shared" si="3"/>
+        <v>8.1498495168699503E-2</v>
+      </c>
+      <c r="F34" s="6">
         <f t="shared" si="1"/>
-        <v>8.1498495168699503E-2</v>
-      </c>
-      <c r="F34" s="6">
-        <f>B34/J34</f>
         <v>1.0326970554585416E-3</v>
       </c>
       <c r="G34" s="2">
         <v>37878</v>
       </c>
       <c r="H34" s="6">
-        <f>G34/J34</f>
+        <f t="shared" si="2"/>
         <v>1.2671363481262922E-2</v>
       </c>
       <c r="I34" s="1">
@@ -1766,18 +1767,18 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="22">
+        <f t="shared" si="3"/>
+        <v>0.10489489844119036</v>
+      </c>
+      <c r="F35" s="6">
         <f t="shared" si="1"/>
-        <v>0.10489489844119036</v>
-      </c>
-      <c r="F35" s="6">
-        <f>B35/J35</f>
         <v>6.8194533880860139E-4</v>
       </c>
       <c r="G35" s="2">
         <v>33872</v>
       </c>
       <c r="H35" s="6">
-        <f>G35/J35</f>
+        <f t="shared" si="2"/>
         <v>6.5012250256473248E-3</v>
       </c>
       <c r="I35" s="1">
@@ -1800,18 +1801,18 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="22">
+        <f t="shared" si="3"/>
+        <v>0.11703958691910499</v>
+      </c>
+      <c r="F36" s="6">
         <f t="shared" si="1"/>
-        <v>0.11703958691910499</v>
-      </c>
-      <c r="F36" s="6">
-        <f>B36/J36</f>
         <v>7.8963114080308908E-4</v>
       </c>
       <c r="G36" s="2">
         <v>33117</v>
       </c>
       <c r="H36" s="6">
-        <f>G36/J36</f>
+        <f t="shared" si="2"/>
         <v>6.746701364802864E-3</v>
       </c>
       <c r="I36" s="1">
@@ -1834,18 +1835,18 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="22">
+        <f t="shared" si="3"/>
+        <v>5.0458857337082469E-2</v>
+      </c>
+      <c r="F37" s="6">
         <f t="shared" si="1"/>
-        <v>5.0458857337082469E-2</v>
-      </c>
-      <c r="F37" s="6">
-        <f>B37/J37</f>
         <v>3.7967128789941339E-4</v>
       </c>
       <c r="G37" s="2">
         <v>32363</v>
       </c>
       <c r="H37" s="6">
-        <f>G37/J37</f>
+        <f t="shared" si="2"/>
         <v>7.5243734784376697E-3</v>
       </c>
       <c r="I37" s="1">
@@ -1868,18 +1869,18 @@
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="22">
+        <f t="shared" si="3"/>
+        <v>4.2070691273068499E-2</v>
+      </c>
+      <c r="F38" s="6">
         <f t="shared" si="1"/>
-        <v>4.2070691273068499E-2</v>
-      </c>
-      <c r="F38" s="6">
-        <f>B38/J38</f>
         <v>6.4150259462759463E-4</v>
       </c>
       <c r="G38" s="2">
         <v>31970</v>
       </c>
       <c r="H38" s="6">
-        <f>G38/J38</f>
+        <f t="shared" si="2"/>
         <v>1.5248206654456654E-2</v>
       </c>
       <c r="I38" s="1">
@@ -1902,18 +1903,18 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="22">
+        <f t="shared" si="3"/>
+        <v>7.7257773532845173E-2</v>
+      </c>
+      <c r="F39" s="6">
         <f t="shared" si="1"/>
-        <v>7.7257773532845173E-2</v>
-      </c>
-      <c r="F39" s="6">
-        <f>B39/J39</f>
         <v>5.5223738318371427E-4</v>
       </c>
       <c r="G39" s="2">
         <v>28269</v>
       </c>
       <c r="H39" s="6">
-        <f>G39/J39</f>
+        <f t="shared" si="2"/>
         <v>7.1479847001924991E-3</v>
       </c>
       <c r="I39" s="1">
@@ -1936,18 +1937,18 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="22">
+        <f t="shared" si="3"/>
+        <v>7.6752988794363458E-2</v>
+      </c>
+      <c r="F40" s="6">
         <f t="shared" si="1"/>
-        <v>7.6752988794363458E-2</v>
-      </c>
-      <c r="F40" s="6">
-        <f>B40/J40</f>
         <v>4.5514226307045015E-4</v>
       </c>
       <c r="G40" s="2">
         <v>26683</v>
       </c>
       <c r="H40" s="6">
-        <f>G40/J40</f>
+        <f t="shared" si="2"/>
         <v>5.9299614284711042E-3</v>
       </c>
       <c r="I40" s="1">
@@ -1970,18 +1971,18 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11582461273020517</v>
       </c>
       <c r="F41" s="6">
-        <f>B41/J41</f>
+        <f t="shared" ref="F41:F60" si="4">B41/J41</f>
         <v>9.835466155867932E-4</v>
       </c>
       <c r="G41" s="2">
         <v>26661</v>
       </c>
       <c r="H41" s="6">
-        <f>G41/J41</f>
+        <f t="shared" ref="H41:H72" si="5">G41/J41</f>
         <v>8.4916892222019081E-3</v>
       </c>
       <c r="I41" s="1">
@@ -2004,18 +2005,18 @@
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14196506550218341</v>
       </c>
       <c r="F42" s="6">
-        <f>B42/J42</f>
+        <f t="shared" si="4"/>
         <v>3.0781291867433089E-3</v>
       </c>
       <c r="G42" s="2">
         <v>22900</v>
       </c>
       <c r="H42" s="6">
-        <f>G42/J42</f>
+        <f t="shared" si="5"/>
         <v>2.1682300331104822E-2</v>
       </c>
       <c r="I42" s="1">
@@ -2038,18 +2039,18 @@
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0039278784723866E-2</v>
       </c>
       <c r="F43" s="6">
-        <f>B43/J43</f>
+        <f t="shared" si="4"/>
         <v>4.870024636401657E-4</v>
       </c>
       <c r="G43" s="2">
         <v>21131</v>
       </c>
       <c r="H43" s="6">
-        <f>G43/J43</f>
+        <f t="shared" si="5"/>
         <v>6.9532763913380691E-3</v>
       </c>
       <c r="I43" s="1">
@@ -2070,18 +2071,18 @@
         <v>504</v>
       </c>
       <c r="E44" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5952626158599383E-2</v>
       </c>
       <c r="F44" s="6">
-        <f>B44/J44</f>
+        <f t="shared" si="4"/>
         <v>3.5676692713955746E-4</v>
       </c>
       <c r="G44" s="2">
         <v>19420</v>
       </c>
       <c r="H44" s="6">
-        <f>G44/J44</f>
+        <f t="shared" si="5"/>
         <v>1.3746852629067869E-2</v>
       </c>
       <c r="I44" s="1">
@@ -2104,18 +2105,18 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1005559968228753</v>
       </c>
       <c r="F45" s="6">
-        <f>B45/J45</f>
+        <f t="shared" si="4"/>
         <v>5.9719816884386647E-4</v>
       </c>
       <c r="G45" s="2">
         <v>18885</v>
       </c>
       <c r="H45" s="6">
-        <f>G45/J45</f>
+        <f t="shared" si="5"/>
         <v>5.9389612525626214E-3</v>
       </c>
       <c r="I45" s="1">
@@ -2136,18 +2137,18 @@
         <v>640</v>
       </c>
       <c r="E46" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.7563094259889657E-2</v>
       </c>
       <c r="F46" s="6">
-        <f>B46/J46</f>
+        <f t="shared" si="4"/>
         <v>3.5994083472529203E-4</v>
       </c>
       <c r="G46" s="2">
         <v>17038</v>
       </c>
       <c r="H46" s="6">
-        <f>G46/J46</f>
+        <f t="shared" si="5"/>
         <v>9.5822999094523839E-3</v>
       </c>
       <c r="I46" s="1">
@@ -2170,18 +2171,18 @@
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.6136032817255523E-2</v>
       </c>
       <c r="F47" s="6">
-        <f>B47/J47</f>
+        <f t="shared" si="4"/>
         <v>7.9566039264991595E-4</v>
       </c>
       <c r="G47" s="2">
         <v>15114</v>
       </c>
       <c r="H47" s="6">
-        <f>G47/J47</f>
+        <f t="shared" si="5"/>
         <v>8.2764013589200491E-3</v>
       </c>
       <c r="I47" s="1">
@@ -2204,18 +2205,18 @@
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10079875591998304</v>
       </c>
       <c r="F48" s="6">
-        <f>B48/J48</f>
+        <f t="shared" si="4"/>
         <v>4.899742540176343E-4</v>
       </c>
       <c r="G48" s="2">
         <v>14147</v>
       </c>
       <c r="H48" s="6">
-        <f>G48/J48</f>
+        <f t="shared" si="5"/>
         <v>4.8609156883502608E-3</v>
       </c>
       <c r="I48" s="1">
@@ -2236,18 +2237,18 @@
         <v>734</v>
       </c>
       <c r="E49" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.9471722573326849E-2</v>
       </c>
       <c r="F49" s="6">
-        <f>B49/J49</f>
+        <f t="shared" si="4"/>
         <v>5.4540455791765433E-4</v>
       </c>
       <c r="G49" s="2">
         <v>12342</v>
       </c>
       <c r="H49" s="6">
-        <f>G49/J49</f>
+        <f t="shared" si="5"/>
         <v>9.1708215992093861E-3</v>
       </c>
       <c r="I49" s="1">
@@ -2270,18 +2271,18 @@
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14312418725617684</v>
       </c>
       <c r="F50" s="6">
-        <f>B50/J50</f>
+        <f t="shared" si="4"/>
         <v>1.7916461066543221E-3</v>
       </c>
       <c r="G50" s="2">
         <v>12304</v>
       </c>
       <c r="H50" s="6">
-        <f>G50/J50</f>
+        <f t="shared" si="5"/>
         <v>1.2518122485107768E-2</v>
       </c>
       <c r="I50" s="1">
@@ -2304,18 +2305,18 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.7855297157622733E-2</v>
       </c>
       <c r="F51" s="6">
-        <f>B51/J51</f>
+        <f t="shared" si="4"/>
         <v>7.4384902490144005E-4</v>
       </c>
       <c r="G51" s="2">
         <v>11610</v>
       </c>
       <c r="H51" s="6">
-        <f>G51/J51</f>
+        <f t="shared" si="5"/>
         <v>8.4667521363781546E-3</v>
       </c>
       <c r="I51" s="1">
@@ -2338,18 +2339,18 @@
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.17867685362042021</v>
       </c>
       <c r="F52" s="6">
-        <f>B52/J52</f>
+        <f t="shared" si="4"/>
         <v>2.8556086067876899E-3</v>
       </c>
       <c r="G52" s="2">
         <v>11518</v>
       </c>
       <c r="H52" s="6">
-        <f>G52/J52</f>
+        <f t="shared" si="5"/>
         <v>1.5981972756550347E-2</v>
       </c>
       <c r="I52" s="1">
@@ -2370,18 +2371,18 @@
         <v>871</v>
       </c>
       <c r="E53" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.6692788588535704E-2</v>
       </c>
       <c r="F53" s="6">
-        <f>B53/J53</f>
+        <f t="shared" si="4"/>
         <v>4.4607875773979933E-4</v>
       </c>
       <c r="G53" s="2">
         <v>11357</v>
       </c>
       <c r="H53" s="6">
-        <f>G53/J53</f>
+        <f t="shared" si="5"/>
         <v>5.8164367986807131E-3</v>
       </c>
       <c r="I53" s="1">
@@ -2402,18 +2403,18 @@
         <v>341</v>
       </c>
       <c r="E54" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.1238548919017957E-2</v>
       </c>
       <c r="F54" s="6">
-        <f>B54/J54</f>
+        <f t="shared" si="4"/>
         <v>4.4766929710669101E-4</v>
       </c>
       <c r="G54" s="2">
         <v>10916</v>
       </c>
       <c r="H54" s="6">
-        <f>G54/J54</f>
+        <f t="shared" si="5"/>
         <v>1.4330668760166096E-2</v>
       </c>
       <c r="I54" s="1">
@@ -2434,18 +2435,18 @@
         <v>752</v>
       </c>
       <c r="E55" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.1043930089749643E-2</v>
       </c>
       <c r="F55" s="6">
-        <f>B55/J55</f>
+        <f t="shared" si="4"/>
         <v>1.1973359275611764E-3</v>
       </c>
       <c r="G55" s="2">
         <v>10585</v>
       </c>
       <c r="H55" s="6">
-        <f>G55/J55</f>
+        <f t="shared" si="5"/>
         <v>1.6853458501642358E-2</v>
       </c>
       <c r="I55" s="1">
@@ -2466,18 +2467,18 @@
         <v>988</v>
       </c>
       <c r="E56" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10628227194492254</v>
       </c>
       <c r="F56" s="6">
-        <f>B56/J56</f>
+        <f t="shared" si="4"/>
         <v>1.0940979616334838E-3</v>
       </c>
       <c r="G56" s="2">
         <v>9296</v>
       </c>
       <c r="H56" s="6">
-        <f>G56/J56</f>
+        <f t="shared" si="5"/>
         <v>1.0294265841442172E-2</v>
       </c>
       <c r="I56" s="1">
@@ -2498,18 +2499,18 @@
         <v>399</v>
       </c>
       <c r="E57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3209876543209874E-2</v>
       </c>
       <c r="F57" s="6">
-        <f>B57/J57</f>
+        <f t="shared" si="4"/>
         <v>3.6714671790157705E-4</v>
       </c>
       <c r="G57" s="2">
         <v>9234</v>
       </c>
       <c r="H57" s="6">
-        <f>G57/J57</f>
+        <f t="shared" si="5"/>
         <v>8.4968240428650692E-3</v>
       </c>
       <c r="I57" s="1">
@@ -2530,18 +2531,18 @@
         <v>285</v>
       </c>
       <c r="E58" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.4139913751796841E-2</v>
       </c>
       <c r="F58" s="6">
-        <f>B58/J58</f>
+        <f t="shared" si="4"/>
         <v>3.8828232075661918E-4</v>
       </c>
       <c r="G58" s="2">
         <v>8348</v>
       </c>
       <c r="H58" s="6">
-        <f>G58/J58</f>
+        <f t="shared" si="5"/>
         <v>1.1373266012899147E-2</v>
       </c>
       <c r="I58" s="1">
@@ -2562,18 +2563,18 @@
         <v>923</v>
       </c>
       <c r="E59" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.12806993201054531</v>
       </c>
       <c r="F59" s="6">
-        <f>B59/J59</f>
+        <f t="shared" si="4"/>
         <v>3.0440295960147289E-4</v>
       </c>
       <c r="G59" s="2">
         <v>7207</v>
       </c>
       <c r="H59" s="6">
-        <f>G59/J59</f>
+        <f t="shared" si="5"/>
         <v>2.3768495447971994E-3</v>
       </c>
       <c r="I59" s="1">
@@ -2594,18 +2595,18 @@
         <v>275</v>
       </c>
       <c r="E60" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6109993293091886E-2</v>
       </c>
       <c r="F60" s="6">
-        <f>B60/J60</f>
+        <f t="shared" si="4"/>
         <v>4.8498743441647196E-4</v>
       </c>
       <c r="G60" s="2">
         <v>5964</v>
       </c>
       <c r="H60" s="6">
-        <f>G60/J60</f>
+        <f t="shared" si="5"/>
         <v>1.0518054759490322E-2</v>
       </c>
       <c r="I60" s="1">

</xml_diff>